<commit_message>
Updates on how poverty tables were calculated
</commit_message>
<xml_diff>
--- a/data/children_in_poverty_200_fpl.xlsx
+++ b/data/children_in_poverty_200_fpl.xlsx
@@ -391,11 +391,11 @@
         </is>
       </c>
       <c r="C2">
-        <v>1.028985507246377</v>
+        <v>0.8652770716827656</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>0.5090579710144928</v>
+        <v>0.6507371631926793</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>1.957971014492754</v>
+        <v>2.153736654804271</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -451,11 +451,11 @@
         </is>
       </c>
       <c r="C5">
-        <v>1.318840579710145</v>
+        <v>1.544483985765124</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>1.540760869565217</v>
+        <v>2.109134045077105</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -491,11 +491,11 @@
         </is>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>1.525165226232842</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -511,11 +511,11 @@
         </is>
       </c>
       <c r="C8">
-        <v>0.6898550724637681</v>
+        <v>1.020640569395018</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Below Median</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>1.855676328502415</v>
+        <v>2.763938315539739</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -551,7 +551,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>0.7608695652173912</v>
+        <v>0.6761565836298933</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -571,11 +571,11 @@
         </is>
       </c>
       <c r="C11">
-        <v>1.00054347826087</v>
+        <v>0.8640569395017794</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -591,11 +591,11 @@
         </is>
       </c>
       <c r="C12">
-        <v>1.032608695652174</v>
+        <v>0.9150991357397052</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>1.087409420289855</v>
+        <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -631,11 +631,11 @@
         </is>
       </c>
       <c r="C14">
-        <v>1.334692028985507</v>
+        <v>1.138790035587189</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -651,11 +651,11 @@
         </is>
       </c>
       <c r="C15">
-        <v>1.458333333333333</v>
+        <v>1.175563463819691</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -671,7 +671,7 @@
         </is>
       </c>
       <c r="C16">
-        <v>0.8293478260869566</v>
+        <v>0.896797153024911</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="C17">
-        <v>0.9146286231884058</v>
+        <v>0.9306049822064056</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="C18">
-        <v>0.5727657004830917</v>
+        <v>0.8125741399762753</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -731,7 +731,7 @@
         </is>
       </c>
       <c r="C19">
-        <v>0.8510466988727858</v>
+        <v>0.8390668248319494</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -751,7 +751,7 @@
         </is>
       </c>
       <c r="C20">
-        <v>0.7059178743961352</v>
+        <v>0.697508896797153</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="C21">
-        <v>0.6518115942028985</v>
+        <v>0.6790035587188612</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="C22">
-        <v>0.5217391304347826</v>
+        <v>0.6456532791052364</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         </is>
       </c>
       <c r="C23">
-        <v>0.6105072463768116</v>
+        <v>0.6751398068124047</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -831,11 +831,11 @@
         </is>
       </c>
       <c r="C24">
-        <v>1.389855072463768</v>
+        <v>1.928825622775801</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>1st Tier</t>
         </is>
       </c>
     </row>
@@ -851,11 +851,11 @@
         </is>
       </c>
       <c r="C25">
-        <v>1.675724637681159</v>
+        <v>1.653279105236401</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -871,11 +871,11 @@
         </is>
       </c>
       <c r="C26">
-        <v>1.361111111111111</v>
+        <v>1.962040332147094</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>1st Tier</t>
         </is>
       </c>
     </row>
@@ -891,11 +891,11 @@
         </is>
       </c>
       <c r="C27">
-        <v>1.499547101449275</v>
+        <v>1.421708185053381</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -911,11 +911,11 @@
         </is>
       </c>
       <c r="C28">
-        <v>1.001811594202898</v>
+        <v>1.405693950177936</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -931,7 +931,7 @@
         </is>
       </c>
       <c r="C29">
-        <v>0.5757246376811593</v>
+        <v>0.706049822064057</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="C30">
-        <v>1.43677536231884</v>
+        <v>1.6355871886121</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -971,7 +971,7 @@
         </is>
       </c>
       <c r="C31">
-        <v>1.059581320450886</v>
+        <v>1.104784499802294</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         </is>
       </c>
       <c r="C32">
-        <v>1.678985507246377</v>
+        <v>1.829181494661922</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1011,11 +1011,11 @@
         </is>
       </c>
       <c r="C33">
-        <v>1.016606280193237</v>
+        <v>0.7995255041518387</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1031,11 +1031,11 @@
         </is>
       </c>
       <c r="C34">
-        <v>0.9710144927536231</v>
+        <v>1.369598373157092</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Below Median</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="C35">
-        <v>0.4839975845410627</v>
+        <v>0.5599051008303678</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1071,7 +1071,7 @@
         </is>
       </c>
       <c r="C36">
-        <v>1.356884057971014</v>
+        <v>1.638027452974072</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1091,7 +1091,7 @@
         </is>
       </c>
       <c r="C37">
-        <v>0.7355072463768115</v>
+        <v>0.6405693950177936</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
         </is>
       </c>
       <c r="C38">
-        <v>1.27536231884058</v>
+        <v>1.275038129130656</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C39">
-        <v>1.306159420289855</v>
+        <v>1.206914082358922</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1151,11 +1151,11 @@
         </is>
       </c>
       <c r="C40">
-        <v>1.151449275362319</v>
+        <v>1.752313167259786</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>1st Tier</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
         </is>
       </c>
       <c r="C41">
-        <v>1.109601449275362</v>
+        <v>1.019572953736655</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1191,7 +1191,7 @@
         </is>
       </c>
       <c r="C42">
-        <v>0.8327294685990339</v>
+        <v>0.9395017793594306</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1211,11 +1211,11 @@
         </is>
       </c>
       <c r="C43">
-        <v>1.534420289855072</v>
+        <v>1.579181494661922</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1231,11 +1231,11 @@
         </is>
       </c>
       <c r="C44">
-        <v>0.8876811594202898</v>
+        <v>1.076027175671304</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Below Median</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1251,11 +1251,11 @@
         </is>
       </c>
       <c r="C45">
-        <v>1.113405797101449</v>
+        <v>1.049110320284698</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
         </is>
       </c>
       <c r="C46">
-        <v>0.601086956521739</v>
+        <v>0.4427046263345196</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1291,7 +1291,7 @@
         </is>
       </c>
       <c r="C47">
-        <v>0.9658816425120773</v>
+        <v>0.8315539739027283</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1311,7 +1311,7 @@
         </is>
       </c>
       <c r="C48">
-        <v>1.185688405797101</v>
+        <v>1.164590747330961</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1331,11 +1331,11 @@
         </is>
       </c>
       <c r="C49">
-        <v>1.41268115942029</v>
+        <v>1.060498220640569</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1351,11 +1351,11 @@
         </is>
       </c>
       <c r="C50">
-        <v>1.071557971014493</v>
+        <v>0.9635231316725978</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>4th Tier</t>
+          <t>Below Median</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
         </is>
       </c>
       <c r="C51">
-        <v>0.8834541062801933</v>
+        <v>0.604982206405694</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C52">
-        <v>0.6644927536231884</v>
+        <v>0.7288256227758008</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1411,11 +1411,11 @@
         </is>
       </c>
       <c r="C53">
-        <v>1.204710144927536</v>
+        <v>1.67497034400949</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>1st Tier</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
         </is>
       </c>
       <c r="C54">
-        <v>0.9035326086956521</v>
+        <v>0.599644128113879</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1451,7 +1451,7 @@
         </is>
       </c>
       <c r="C55">
-        <v>1.123188405797101</v>
+        <v>1.234367056431113</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1471,7 +1471,7 @@
         </is>
       </c>
       <c r="C56">
-        <v>0.9184782608695652</v>
+        <v>0.8784951703101169</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="C57">
-        <v>0.527536231884058</v>
+        <v>0.8042704626334519</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1511,7 +1511,7 @@
         </is>
       </c>
       <c r="C58">
-        <v>0.6124999999999999</v>
+        <v>0.5701067615658363</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         </is>
       </c>
       <c r="C59">
-        <v>0.3043478260869565</v>
+        <v>0.2740213523131673</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1551,7 +1551,7 @@
         </is>
       </c>
       <c r="C60">
-        <v>0.5126811594202898</v>
+        <v>0.523640061006609</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1571,11 +1571,11 @@
         </is>
       </c>
       <c r="C61">
-        <v>0.8211050724637681</v>
+        <v>1.238434163701068</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Below Median</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1591,11 +1591,11 @@
         </is>
       </c>
       <c r="C62">
-        <v>1.341032608695652</v>
+        <v>1.921708185053381</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>1st Tier</t>
         </is>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
         </is>
       </c>
       <c r="C63">
-        <v>0.6391304347826087</v>
+        <v>0.6818505338078291</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="C64">
-        <v>0.5807971014492753</v>
+        <v>0.6220640569395018</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="C65">
-        <v>0.6625905797101449</v>
+        <v>0.6423487544483986</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="C66">
-        <v>0.3719806763285024</v>
+        <v>0.6749703440094899</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1691,11 +1691,11 @@
         </is>
       </c>
       <c r="C67">
-        <v>0.9739130434782608</v>
+        <v>1.268327402135231</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Below Median</t>
+          <t>3rd Tier</t>
         </is>
       </c>
     </row>
@@ -1711,11 +1711,11 @@
         </is>
       </c>
       <c r="C68">
-        <v>1.911684782608696</v>
+        <v>1.421708185053381</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
         </is>
       </c>
       <c r="C69">
-        <v>0.6036231884057971</v>
+        <v>0.4498220640569395</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="C70">
-        <v>0.8876811594202898</v>
+        <v>0.8042704626334519</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1771,11 +1771,11 @@
         </is>
       </c>
       <c r="C71">
-        <v>1.607971014492753</v>
+        <v>1.134519572953737</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1791,11 +1791,11 @@
         </is>
       </c>
       <c r="C72">
-        <v>1.557246376811594</v>
+        <v>1.412099644128114</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1st Tier</t>
+          <t>2nd Tier</t>
         </is>
       </c>
     </row>
@@ -1811,7 +1811,7 @@
         </is>
       </c>
       <c r="C73">
-        <v>0.5427536231884057</v>
+        <v>0.604982206405694</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -1831,7 +1831,7 @@
         </is>
       </c>
       <c r="C74">
-        <v>1.327898550724637</v>
+        <v>1.218098627351296</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1851,11 +1851,11 @@
         </is>
       </c>
       <c r="C75">
-        <v>1.296014492753623</v>
+        <v>2.542348754448398</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>3rd Tier</t>
+          <t>1st Tier</t>
         </is>
       </c>
     </row>
@@ -1871,11 +1871,11 @@
         </is>
       </c>
       <c r="C76">
-        <v>1.348429951690821</v>
+        <v>1.111506524317912</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2nd Tier</t>
+          <t>4th Tier</t>
         </is>
       </c>
     </row>
@@ -1891,7 +1891,7 @@
         </is>
       </c>
       <c r="C77">
-        <v>0.7684782608695652</v>
+        <v>0.7871886120996441</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="C78">
-        <v>1.480525362318841</v>
+        <v>1.50711743772242</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -1931,7 +1931,7 @@
         </is>
       </c>
       <c r="C79">
-        <v>0.6657608695652174</v>
+        <v>0.603202846975089</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -1951,7 +1951,7 @@
         </is>
       </c>
       <c r="C80">
-        <v>0.6467391304347826</v>
+        <v>0.8291814946619217</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>

</xml_diff>